<commit_message>
added precision and graphcs
</commit_message>
<xml_diff>
--- a/relationFlows.xlsx
+++ b/relationFlows.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\Organizer\School\BachelorProject\GroundedTheory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\Organizer\School\BachelorProject\GroundedTheoryDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC6D8E4-8100-4C7E-8EDB-0DA2F4EC635E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCC754C-EBE4-48CA-972C-0420524DCDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6840" windowWidth="16440" windowHeight="28440" tabRatio="761" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="33" r:id="rId1"/>
@@ -1255,23 +1255,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>599962</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>116540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>599964</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>60966</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Arrow: Down 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF907F41-FCA6-4CF7-878A-73CD68C4BBB8}"/>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7622</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>73966</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Arrow: Down 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B56F9F9E-5E81-4E6F-A66A-C7D8FF0B7C71}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1279,7 +1279,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="1359270" y="14170512"/>
+          <a:off x="1376528" y="9794392"/>
           <a:ext cx="310186" cy="1828802"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -1310,205 +1310,6 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-NL" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>7622</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>73966</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Arrow: Down 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B56F9F9E-5E81-4E6F-A66A-C7D8FF0B7C71}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000">
-          <a:off x="1376528" y="9794392"/>
-          <a:ext cx="310186" cy="1828802"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 21246"/>
-            <a:gd name="adj2" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-NL" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>313764</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>143435</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>92784</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>130884</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Flowchart: Alternate Process 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A563F72B-218B-40E1-9DFD-0526F49579E7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="923364" y="14773835"/>
-          <a:ext cx="998220" cy="536089"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartAlternateProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Builds / continues</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> on</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-NL" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>466164</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>112955</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>245184</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>100404</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Flowchart: Alternate Process 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE23BEC-A0CB-4FF1-908B-445BCD0C3AE3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1075764" y="14926235"/>
-          <a:ext cx="998220" cy="536089"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartAlternateProcess">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Builds / continues</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> on</a:t>
-          </a:r>
           <a:endParaRPr lang="en-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -9404,7 +9205,7 @@
   <dimension ref="B2:H60"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9507,7 +9308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305519BB-09CB-4B9E-9AF5-8616065EDC97}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
@@ -9570,7 +9371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0CFC38-9D88-498C-8541-194B92CA9E23}">
   <dimension ref="B1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -9602,7 +9403,7 @@
   <dimension ref="B1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9665,8 +9466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9687,7 +9488,7 @@
   <dimension ref="B1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9770,7 +9571,7 @@
   <dimension ref="B1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K36" sqref="A1:XFD1048576"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9790,7 +9591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70D9D27-8121-4A58-94E2-2D33AF54AD1E}">
   <dimension ref="B1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added new excel containing unique_pairs and chi squared test
</commit_message>
<xml_diff>
--- a/relationFlows.xlsx
+++ b/relationFlows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\Organizer\School\BachelorProject\GroundedTheoryDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE36EDB-9B3F-44CF-B89D-1DAEC8C6E0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96D5164-1498-422E-B0E5-111DD0BE36FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="761" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pattern6" sheetId="26" r:id="rId1"/>
@@ -4748,8 +4748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB2C13A-6C31-4A67-A527-41C03E4091AE}">
   <dimension ref="B2:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4864,7 +4864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
@@ -4907,7 +4907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305519BB-09CB-4B9E-9AF5-8616065EDC97}">
   <dimension ref="B1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
@@ -4939,7 +4939,7 @@
   <dimension ref="B1"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>